<commit_message>
Updated spreadsheet to match feedback
</commit_message>
<xml_diff>
--- a/DFS/DFS Documentation - Jonathan Sarasua.xlsx
+++ b/DFS/DFS Documentation - Jonathan Sarasua.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Guildhall\DFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE829CD5-19C4-4766-8F30-AADBDF50DC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9744D6-ABA9-415F-B9C2-C0887F13BFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C664E016-CE9A-4FC5-A772-98B630577C19}"/>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{45A633AA-53D9-4A86-8576-B3408263D8D7}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{C664E016-CE9A-4FC5-A772-98B630577C19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3D84B222-422C-4254-85C9-E5FC35CCD999}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="209">
   <si>
     <t>Fields</t>
   </si>
@@ -106,18 +106,6 @@
     <t>Background</t>
   </si>
   <si>
-    <t>Data driven Weapons</t>
-  </si>
-  <si>
-    <t>Data driven Bullets</t>
-  </si>
-  <si>
-    <t>Weapons are data driven with Weapon visual, VFX, and SFX</t>
-  </si>
-  <si>
-    <t>Bullets are data driven with damage, visuals, VFX, and SFX</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -289,9 +277,6 @@
     <t>Enemies</t>
   </si>
   <si>
-    <t>Enemies are actors with data driven types. They have on hit and on death effects to drop loot</t>
-  </si>
-  <si>
     <t>Enemy Controller</t>
   </si>
   <si>
@@ -638,6 +623,48 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Bullets</t>
+  </si>
+  <si>
+    <t>Weapons may be data driven with Weapon visual, VFX, and SFX</t>
+  </si>
+  <si>
+    <t>Bullets may be data driven with damage, visuals, VFX, and SFX</t>
+  </si>
+  <si>
+    <t>Change documentation to reflect mmoving data driving out of milestone 1</t>
+  </si>
+  <si>
+    <t>Create Prototype player</t>
+  </si>
+  <si>
+    <t>Create prototype gun</t>
+  </si>
+  <si>
+    <t>Create Prototype bullets/firing</t>
+  </si>
+  <si>
+    <t>Enemies are actors that may be data driven. They have on hit and on death effects to drop loot</t>
+  </si>
+  <si>
+    <t>*0</t>
+  </si>
+  <si>
+    <t>Create Protogame as starting place</t>
+  </si>
+  <si>
+    <t>Protogame</t>
+  </si>
+  <si>
+    <t>Create Protogame as starting point</t>
+  </si>
+  <si>
+    <t>Create simple Enemy character with functions to shoot</t>
+  </si>
+  <si>
+    <t>*I</t>
   </si>
 </sst>
 </file>
@@ -693,7 +720,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -799,11 +826,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -820,6 +858,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,8 +900,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE8E595B-F667-4157-9489-6674872D5FB0}" name="Table1" displayName="Table1" ref="A12:E48" totalsRowShown="0">
-  <autoFilter ref="A12:E48" xr:uid="{405829D9-14E9-4F75-A8FD-B274F101C96F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE8E595B-F667-4157-9489-6674872D5FB0}" name="Table1" displayName="Table1" ref="A12:E49" totalsRowShown="0">
+  <autoFilter ref="A12:E49" xr:uid="{405829D9-14E9-4F75-A8FD-B274F101C96F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EE2B776A-53E2-4052-8C41-F2866817EAD3}" name="Feature Id"/>
     <tableColumn id="2" xr3:uid="{09B1D195-814B-4452-B5A6-A2BC7F5A99BB}" name="Game State"/>
@@ -923,8 +962,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AFC5965-674A-4451-AC25-19E71FAB4844}" name="Table35" displayName="Table35" ref="A11:J72" totalsRowCount="1">
-  <autoFilter ref="A11:J71" xr:uid="{4A443AB6-A518-4003-A068-759E12CFD484}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AFC5965-674A-4451-AC25-19E71FAB4844}" name="Table35" displayName="Table35" ref="A11:J77" totalsRowCount="1">
+  <autoFilter ref="A11:J76" xr:uid="{4A443AB6-A518-4003-A068-759E12CFD484}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:J71">
     <sortCondition ref="F11:F71"/>
   </sortState>
@@ -957,22 +996,30 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4151FFFD-B746-4538-A0CE-AB3ABE724425}" name="Table356" displayName="Table356" ref="A17:J43" totalsRowCount="1">
-  <autoFilter ref="A17:J42" xr:uid="{7D17F18C-C430-4F21-9230-429FFCB76917}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:J42">
-    <sortCondition ref="F11:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4151FFFD-B746-4538-A0CE-AB3ABE724425}" name="Table356" displayName="Table356" ref="A17:J38" totalsRowCount="1">
+  <autoFilter ref="A17:J37" xr:uid="{7D17F18C-C430-4F21-9230-429FFCB76917}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:J37">
+    <sortCondition ref="F11:F37"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{62B84147-86F3-475B-86AF-B1B525EF17F5}" name="Task ID"/>
-    <tableColumn id="9" xr3:uid="{04DB83DD-6041-463A-91B0-CD2D2B02A51C}" name="Status"/>
+    <tableColumn id="9" xr3:uid="{04DB83DD-6041-463A-91B0-CD2D2B02A51C}" name="Status">
+      <calculatedColumnFormula>VLOOKUP($A18,Table35[#All],2,TRUE)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="2" xr3:uid="{66E4FD19-F3D8-4D4E-8B75-D158D7160B69}" name="Estimate" totalsRowFunction="custom">
+      <calculatedColumnFormula>VLOOKUP($A18,Table35[#All],3,TRUE)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table356[Estimate])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{6736C0BF-FD3D-4FAC-905E-4D3E13CD53DE}" name="Actual" totalsRowFunction="custom">
+      <calculatedColumnFormula>VLOOKUP($A18,Table35[#All],4,TRUE)</calculatedColumnFormula>
       <totalsRowFormula>SUM(Table356[Actual])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{41F6EB5E-2051-4346-B074-A312A593B6CE}" name="Task"/>
-    <tableColumn id="4" xr3:uid="{CF2678FC-CD55-4A5C-BDFF-B2D47422F0AE}" name="Feature ID"/>
+    <tableColumn id="11" xr3:uid="{41F6EB5E-2051-4346-B074-A312A593B6CE}" name="Task">
+      <calculatedColumnFormula>VLOOKUP($A18,Table35[#All],5,TRUE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{CF2678FC-CD55-4A5C-BDFF-B2D47422F0AE}" name="Feature ID">
+      <calculatedColumnFormula>VLOOKUP($A18,Table35[#All],6,TRUE)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" xr3:uid="{0C1DC99C-3562-42F4-872D-D0D85E3C0C2A}" name="Game State">
       <calculatedColumnFormula>VLOOKUP($F18,Table1[],2,TRUE)</calculatedColumnFormula>
     </tableColumn>
@@ -991,10 +1038,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{618CE7E4-5ADE-4E98-B2AC-0682EBACB73D}" name="Table3567" displayName="Table3567" ref="A47:J49" insertRow="1" totalsRowCount="1">
-  <autoFilter ref="A47:J48" xr:uid="{DD29A22F-BB19-4ADC-B414-52C64CAC47C4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A48:J48">
-    <sortCondition ref="F11:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{618CE7E4-5ADE-4E98-B2AC-0682EBACB73D}" name="Table3567" displayName="Table3567" ref="A42:J44" insertRow="1" totalsRowCount="1">
+  <autoFilter ref="A42:J43" xr:uid="{DD29A22F-BB19-4ADC-B414-52C64CAC47C4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:J43">
+    <sortCondition ref="F11:F37"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{C6F19666-4430-4172-9EF5-7BF02339E0BE}" name="Task ID"/>
@@ -1008,16 +1055,16 @@
     <tableColumn id="11" xr3:uid="{49D5F43A-A98B-42E6-ACBC-67D28734B648}" name="Task"/>
     <tableColumn id="4" xr3:uid="{E8FD2575-FD87-4AEC-B082-FC9EF15436ED}" name="Feature ID"/>
     <tableColumn id="5" xr3:uid="{00E2B42D-24A6-4373-8A60-41DF03320438}" name="Game State">
-      <calculatedColumnFormula>VLOOKUP($F48,Table1[],2,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F43,Table1[],2,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{7CAF72B6-3BE7-4219-8CBF-3144E50061D4}" name="Area">
-      <calculatedColumnFormula>VLOOKUP($F48,Table1[],3,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F43,Table1[],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{006D294A-1C72-4BE8-93FB-F3D69846DA4B}" name="Features">
-      <calculatedColumnFormula>VLOOKUP($F48,Table1[],4,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F43,Table1[],4,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{34E05C3D-FA28-4EB6-94EB-403D79C130C2}" name="Description">
-      <calculatedColumnFormula>VLOOKUP($F48,Table1[],5,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F43,Table1[],5,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1025,10 +1072,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A50E57C5-0AFB-4BA1-ADB8-B627D629FE7F}" name="Table35678" displayName="Table35678" ref="A52:J54" insertRow="1" totalsRowCount="1">
-  <autoFilter ref="A52:J53" xr:uid="{12F7B163-3DD2-4A1A-B717-142A2F111DBF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:J53">
-    <sortCondition ref="F11:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A50E57C5-0AFB-4BA1-ADB8-B627D629FE7F}" name="Table35678" displayName="Table35678" ref="A47:J49" insertRow="1" totalsRowCount="1">
+  <autoFilter ref="A47:J48" xr:uid="{12F7B163-3DD2-4A1A-B717-142A2F111DBF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A48:J48">
+    <sortCondition ref="F11:F37"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{F8381028-8A17-4B32-A639-67E8C8144828}" name="Task ID"/>
@@ -1042,16 +1089,16 @@
     <tableColumn id="11" xr3:uid="{91CFC98B-90CD-42BE-9A24-77BC97E0454A}" name="Task"/>
     <tableColumn id="4" xr3:uid="{B7F5769E-B85A-43C1-902D-895944D9FB69}" name="Feature ID"/>
     <tableColumn id="5" xr3:uid="{B24C2F29-63F0-444C-BEF7-9A76FCB32652}" name="Game State">
-      <calculatedColumnFormula>VLOOKUP($F53,Table1[],2,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F48,Table1[],2,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{FE8182AE-9790-4939-8FF4-6070CF1562BE}" name="Area">
-      <calculatedColumnFormula>VLOOKUP($F53,Table1[],3,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F48,Table1[],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{E7F548A7-6336-48B8-A133-B7FCEE2A2BDE}" name="Features">
-      <calculatedColumnFormula>VLOOKUP($F53,Table1[],4,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F48,Table1[],4,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{FA6C449C-FC00-4EF7-B313-44A06BA6C8C8}" name="Description">
-      <calculatedColumnFormula>VLOOKUP($F53,Table1[],5,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F48,Table1[],5,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1059,10 +1106,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{30F3182D-6F4F-47DA-9031-C4C7700B24D0}" name="Table356789" displayName="Table356789" ref="A57:J59" insertRow="1" totalsRowCount="1">
-  <autoFilter ref="A57:J58" xr:uid="{B94650E2-40D2-4E6D-BDD5-60BDE959C1FE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A58:J58">
-    <sortCondition ref="F11:F42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{30F3182D-6F4F-47DA-9031-C4C7700B24D0}" name="Table356789" displayName="Table356789" ref="A52:J54" insertRow="1" totalsRowCount="1">
+  <autoFilter ref="A52:J53" xr:uid="{B94650E2-40D2-4E6D-BDD5-60BDE959C1FE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:J53">
+    <sortCondition ref="F11:F37"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{DC6AA35E-8AA3-446B-B599-609F1953960A}" name="Task ID"/>
@@ -1076,16 +1123,16 @@
     <tableColumn id="11" xr3:uid="{F62C4925-2A4F-4E55-8ABC-E6F6593114DC}" name="Task"/>
     <tableColumn id="4" xr3:uid="{01A791A3-ACBC-4A55-B3B0-A86AD9A448A7}" name="Feature ID"/>
     <tableColumn id="5" xr3:uid="{295C0FE1-E8EF-4354-AFB2-7D7ABA42869A}" name="Game State">
-      <calculatedColumnFormula>VLOOKUP($F58,Table1[],2,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F53,Table1[],2,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{FF2F79F8-5BB6-4B43-A8B1-9663B716C6B1}" name="Area">
-      <calculatedColumnFormula>VLOOKUP($F58,Table1[],3,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F53,Table1[],3,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{5482843D-6E87-4AC9-93CD-093636B159C7}" name="Features">
-      <calculatedColumnFormula>VLOOKUP($F58,Table1[],4,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F53,Table1[],4,TRUE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{677E5A6C-8291-472B-8F25-DC573BD78CC5}" name="Description">
-      <calculatedColumnFormula>VLOOKUP($F58,Table1[],5,TRUE)</calculatedColumnFormula>
+      <calculatedColumnFormula>VLOOKUP($F53,Table1[],5,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1400,12 +1447,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CAAFA2-F5E8-420F-97C9-09E9E707D7A4}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A16" workbookViewId="1">
+      <selection activeCell="E51" sqref="E51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1430,7 +1479,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1440,10 +1489,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1524,7 +1573,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,7 +1607,7 @@
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1572,7 +1621,7 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1589,10 +1638,10 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,10 +1655,10 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>195</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1620,13 +1669,13 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1637,13 +1686,13 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,13 +1703,13 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1671,13 +1720,13 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,13 +1737,13 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1705,13 +1754,13 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1722,13 +1771,13 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,16 +1785,16 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,13 +1805,13 @@
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,13 +1822,13 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,13 +1839,13 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
         <v>47</v>
-      </c>
-      <c r="D31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,13 +1856,13 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1824,13 +1873,13 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,13 +1890,13 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,13 +1907,13 @@
         <v>9</v>
       </c>
       <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="s">
         <v>68</v>
-      </c>
-      <c r="D35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E35" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,13 +1924,13 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,13 +1941,13 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,13 +1958,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1926,13 +1975,13 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1943,13 +1992,13 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,13 +2009,13 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1974,16 +2023,16 @@
         <v>30</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1994,13 +2043,13 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2011,13 +2060,13 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" t="s">
         <v>56</v>
-      </c>
-      <c r="D44" t="s">
-        <v>59</v>
-      </c>
-      <c r="E44" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2028,13 +2077,13 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,13 +2094,13 @@
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,13 +2111,13 @@
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2076,16 +2125,33 @@
         <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2100,12 +2166,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAEC069-D6F8-4CCE-BE78-F924E31A4A35}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="1">
-      <selection activeCell="B46" sqref="B46"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2128,15 +2192,15 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2">
         <v>43997</v>
@@ -2144,7 +2208,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B8" s="2">
         <v>44011</v>
@@ -2152,7 +2216,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2">
         <v>44025</v>
@@ -2160,7 +2224,7 @@
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2">
         <v>44033</v>
@@ -2172,10 +2236,10 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -2192,7 +2256,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <v>36</v>
@@ -2216,7 +2280,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2240,7 +2304,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2264,7 +2328,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -2288,7 +2352,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -2303,16 +2367,16 @@
       </c>
       <c r="E17" t="str">
         <f>VLOOKUP($B17,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="F17" t="str">
         <f>VLOOKUP($B17,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -2327,16 +2391,16 @@
       </c>
       <c r="E18" t="str">
         <f>VLOOKUP($B18,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Bullets</v>
       </c>
       <c r="F18" t="str">
         <f>VLOOKUP($B18,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -2360,7 +2424,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B20">
         <v>17</v>
@@ -2384,7 +2448,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B21">
         <v>18</v>
@@ -2408,7 +2472,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22">
         <v>19</v>
@@ -2432,7 +2496,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -2456,7 +2520,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B24">
         <v>21</v>
@@ -2480,7 +2544,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B25">
         <v>22</v>
@@ -2504,7 +2568,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B26">
         <v>23</v>
@@ -2528,7 +2592,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2552,7 +2616,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B28">
         <v>11</v>
@@ -2576,7 +2640,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B29">
         <v>13</v>
@@ -2600,7 +2664,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B30">
         <v>24</v>
@@ -2624,7 +2688,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B31">
         <v>25</v>
@@ -2648,7 +2712,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B32">
         <v>26</v>
@@ -2672,7 +2736,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>27</v>
@@ -2691,12 +2755,12 @@
       </c>
       <c r="F33" t="str">
         <f>VLOOKUP($B33,Table1[],5,TRUE)</f>
-        <v>Enemies are actors with data driven types. They have on hit and on death effects to drop loot</v>
+        <v>Enemies are actors that may be data driven. They have on hit and on death effects to drop loot</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B34">
         <v>31</v>
@@ -2720,7 +2784,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B35">
         <v>32</v>
@@ -2744,7 +2808,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B36">
         <v>33</v>
@@ -2768,7 +2832,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B37">
         <v>34</v>
@@ -2792,7 +2856,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B38">
         <v>35</v>
@@ -2816,7 +2880,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -2840,7 +2904,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -2864,7 +2928,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B41">
         <v>6</v>
@@ -2888,7 +2952,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B42">
         <v>12</v>
@@ -2912,7 +2976,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B43">
         <v>14</v>
@@ -2936,7 +3000,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B44">
         <v>15</v>
@@ -2960,7 +3024,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B45">
         <v>16</v>
@@ -2984,7 +3048,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B46">
         <v>28</v>
@@ -3008,7 +3072,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B47">
         <v>29</v>
@@ -3032,7 +3096,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B48">
         <v>30</v>
@@ -3067,13 +3131,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC20C21-6CC5-454B-A71B-54C5FBC17A7F}">
-  <dimension ref="A2:J72"/>
+  <dimension ref="A2:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A49" workbookViewId="1">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,93 +3153,93 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -3204,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3240,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -3276,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -3312,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -3348,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -3384,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -3420,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F18">
         <v>6</v>
@@ -3446,8 +3510,8 @@
       <c r="A19">
         <v>8</v>
       </c>
-      <c r="B19">
-        <v>0</v>
+      <c r="B19" t="s">
+        <v>112</v>
       </c>
       <c r="C19">
         <v>1.5</v>
@@ -3456,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F19">
         <v>7</v>
@@ -3471,19 +3535,19 @@
       </c>
       <c r="I19" t="str">
         <f>VLOOKUP($F19,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J19" t="str">
         <f>VLOOKUP($F19,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" t="s">
+        <v>112</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3492,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F20">
         <v>7</v>
@@ -3507,11 +3571,11 @@
       </c>
       <c r="I20" t="str">
         <f>VLOOKUP($F20,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J20" t="str">
         <f>VLOOKUP($F20,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3528,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F21">
         <v>7</v>
@@ -3543,11 +3607,11 @@
       </c>
       <c r="I21" t="str">
         <f>VLOOKUP($F21,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J21" t="str">
         <f>VLOOKUP($F21,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3564,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F22">
         <v>7</v>
@@ -3579,11 +3643,11 @@
       </c>
       <c r="I22" t="str">
         <f>VLOOKUP($F22,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J22" t="str">
         <f>VLOOKUP($F22,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3600,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F23">
         <v>7</v>
@@ -3615,11 +3679,11 @@
       </c>
       <c r="I23" t="str">
         <f>VLOOKUP($F23,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J23" t="str">
         <f>VLOOKUP($F23,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3636,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F24">
         <v>7</v>
@@ -3651,11 +3715,11 @@
       </c>
       <c r="I24" t="str">
         <f>VLOOKUP($F24,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J24" t="str">
         <f>VLOOKUP($F24,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3672,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F25">
         <v>7</v>
@@ -3687,11 +3751,11 @@
       </c>
       <c r="I25" t="str">
         <f>VLOOKUP($F25,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J25" t="str">
         <f>VLOOKUP($F25,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3708,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F26">
         <v>7</v>
@@ -3723,11 +3787,11 @@
       </c>
       <c r="I26" t="str">
         <f>VLOOKUP($F26,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J26" t="str">
         <f>VLOOKUP($F26,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3744,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F27">
         <v>7</v>
@@ -3759,19 +3823,19 @@
       </c>
       <c r="I27" t="str">
         <f>VLOOKUP($F27,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J27" t="str">
         <f>VLOOKUP($F27,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>17</v>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" t="s">
+        <v>112</v>
       </c>
       <c r="C28">
         <v>1.5</v>
@@ -3780,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F28">
         <v>8</v>
@@ -3795,17 +3859,20 @@
       </c>
       <c r="I28" t="str">
         <f>VLOOKUP($F28,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Bullets</v>
       </c>
       <c r="J28" t="str">
         <f>VLOOKUP($F28,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>18</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
       <c r="C29">
         <v>1</v>
       </c>
@@ -3813,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F29">
         <v>8</v>
@@ -3828,11 +3895,11 @@
       </c>
       <c r="I29" t="str">
         <f>VLOOKUP($F29,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Bullets</v>
       </c>
       <c r="J29" t="str">
         <f>VLOOKUP($F29,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3849,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F30">
         <v>8</v>
@@ -3864,11 +3931,11 @@
       </c>
       <c r="I30" t="str">
         <f>VLOOKUP($F30,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Bullets</v>
       </c>
       <c r="J30" t="str">
         <f>VLOOKUP($F30,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3885,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F31">
         <v>8</v>
@@ -3900,11 +3967,11 @@
       </c>
       <c r="I31" t="str">
         <f>VLOOKUP($F31,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Bullets</v>
       </c>
       <c r="J31" t="str">
         <f>VLOOKUP($F31,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3921,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F32">
         <v>9</v>
@@ -3947,6 +4014,9 @@
       <c r="A33">
         <v>22</v>
       </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
       <c r="C33">
         <v>0.5</v>
       </c>
@@ -3954,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F33">
         <v>9</v>
@@ -3990,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F34">
         <v>10</v>
@@ -4026,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F35">
         <v>11</v>
@@ -4062,7 +4132,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F36">
         <v>12</v>
@@ -4098,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F37">
         <v>13</v>
@@ -4134,7 +4204,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F38">
         <v>14</v>
@@ -4170,7 +4240,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F39">
         <v>15</v>
@@ -4206,7 +4276,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F40">
         <v>16</v>
@@ -4242,7 +4312,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F41">
         <v>17</v>
@@ -4278,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F42">
         <v>18</v>
@@ -4314,7 +4384,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F43">
         <v>18</v>
@@ -4340,8 +4410,8 @@
       <c r="A44">
         <v>33</v>
       </c>
-      <c r="B44">
-        <v>0</v>
+      <c r="B44" t="s">
+        <v>112</v>
       </c>
       <c r="C44">
         <v>1.5</v>
@@ -4350,7 +4420,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F44">
         <v>19</v>
@@ -4386,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F45">
         <v>19</v>
@@ -4422,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F46">
         <v>20</v>
@@ -4458,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F47">
         <v>21</v>
@@ -4494,7 +4564,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F48">
         <v>21</v>
@@ -4530,7 +4600,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F49">
         <v>22</v>
@@ -4566,7 +4636,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F50">
         <v>23</v>
@@ -4602,7 +4672,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F51">
         <v>24</v>
@@ -4638,7 +4708,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F52">
         <v>25</v>
@@ -4674,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F53">
         <v>26</v>
@@ -4710,7 +4780,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F54">
         <v>27</v>
@@ -4729,7 +4799,7 @@
       </c>
       <c r="J54" t="str">
         <f>VLOOKUP($F54,Table1[],5,TRUE)</f>
-        <v>Enemies are actors with data driven types. They have on hit and on death effects to drop loot</v>
+        <v>Enemies are actors that may be data driven. They have on hit and on death effects to drop loot</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -4746,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F55">
         <v>28</v>
@@ -4782,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F56">
         <v>28</v>
@@ -4818,7 +4888,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F57">
         <v>29</v>
@@ -4854,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F58">
         <v>29</v>
@@ -4890,7 +4960,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F59">
         <v>29</v>
@@ -4926,7 +4996,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F60">
         <v>30</v>
@@ -4962,7 +5032,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F61">
         <v>31</v>
@@ -4998,7 +5068,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F62">
         <v>32</v>
@@ -5034,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F63">
         <v>33</v>
@@ -5070,7 +5140,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F64">
         <v>33</v>
@@ -5106,7 +5176,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F65">
         <v>33</v>
@@ -5142,7 +5212,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F66">
         <v>34</v>
@@ -5178,7 +5248,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F67">
         <v>34</v>
@@ -5214,7 +5284,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F68">
         <v>34</v>
@@ -5250,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F69">
         <v>34</v>
@@ -5277,16 +5347,16 @@
         <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>188</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
+        <v>183</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
       </c>
       <c r="D70">
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F70">
         <v>35</v>
@@ -5322,7 +5392,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F71">
         <v>36</v>
@@ -5345,11 +5415,191 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>61</v>
+      </c>
+      <c r="B72" t="s">
+        <v>203</v>
+      </c>
       <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>199</v>
+      </c>
+      <c r="F72">
+        <v>20</v>
+      </c>
+      <c r="G72" t="str">
+        <f>VLOOKUP($F72,Table1[],2,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="H72" t="str">
+        <f>VLOOKUP($F72,Table1[],3,TRUE)</f>
+        <v>Player</v>
+      </c>
+      <c r="I72" t="str">
+        <f>VLOOKUP($F72,Table1[],4,TRUE)</f>
+        <v>Player Character</v>
+      </c>
+      <c r="J72" t="str">
+        <f>VLOOKUP($F72,Table1[],5,TRUE)</f>
+        <v>The Player character is derived from actor with a player controller</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>62</v>
+      </c>
+      <c r="B73" t="s">
+        <v>203</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>200</v>
+      </c>
+      <c r="F73">
+        <v>7</v>
+      </c>
+      <c r="G73" t="str">
+        <f>VLOOKUP($F73,Table1[],2,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="H73" t="str">
+        <f>VLOOKUP($F73,Table1[],3,TRUE)</f>
+        <v>Weapons</v>
+      </c>
+      <c r="I73" t="str">
+        <f>VLOOKUP($F73,Table1[],4,TRUE)</f>
+        <v>Weapons</v>
+      </c>
+      <c r="J73" t="str">
+        <f>VLOOKUP($F73,Table1[],5,TRUE)</f>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>63</v>
+      </c>
+      <c r="B74" t="s">
+        <v>203</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>201</v>
+      </c>
+      <c r="F74">
+        <v>8</v>
+      </c>
+      <c r="G74" t="str">
+        <f>VLOOKUP($F74,Table1[],2,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="H74" t="str">
+        <f>VLOOKUP($F74,Table1[],3,TRUE)</f>
+        <v>Weapons</v>
+      </c>
+      <c r="I74" t="str">
+        <f>VLOOKUP($F74,Table1[],4,TRUE)</f>
+        <v>Bullets</v>
+      </c>
+      <c r="J74" t="str">
+        <f>VLOOKUP($F74,Table1[],5,TRUE)</f>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>207</v>
+      </c>
+      <c r="F75">
+        <v>27</v>
+      </c>
+      <c r="G75" t="str">
+        <f>VLOOKUP($F75,Table1[],2,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="H75" t="str">
+        <f>VLOOKUP($F75,Table1[],3,TRUE)</f>
+        <v>Enemies</v>
+      </c>
+      <c r="I75" t="str">
+        <f>VLOOKUP($F75,Table1[],4,TRUE)</f>
+        <v>Enemy characters</v>
+      </c>
+      <c r="J75" t="str">
+        <f>VLOOKUP($F75,Table1[],5,TRUE)</f>
+        <v>Enemies are actors that may be data driven. They have on hit and on death effects to drop loot</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>65</v>
+      </c>
+      <c r="B76" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>204</v>
+      </c>
+      <c r="F76">
+        <v>37</v>
+      </c>
+      <c r="G76" t="str">
+        <f>VLOOKUP($F76,Table1[],2,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="H76" t="str">
+        <f>VLOOKUP($F76,Table1[],3,TRUE)</f>
+        <v>Protogame</v>
+      </c>
+      <c r="I76" t="str">
+        <f>VLOOKUP($F76,Table1[],4,TRUE)</f>
+        <v>Protogame</v>
+      </c>
+      <c r="J76" t="str">
+        <f>VLOOKUP($F76,Table1[],5,TRUE)</f>
+        <v>Create Protogame as starting point</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C77">
         <f>SUM(Table35[Estimate])</f>
-        <v>101</v>
-      </c>
-      <c r="D72">
+        <v>105</v>
+      </c>
+      <c r="D77">
         <f>SUM(Table35[Actual])</f>
         <v>0</v>
       </c>
@@ -5364,13 +5614,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93182A32-9B41-4840-9B31-4DBA5186CB78}">
-  <dimension ref="A6:J59"/>
+  <dimension ref="A6:J54"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:J18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
-    <sheetView topLeftCell="A10" workbookViewId="1">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A13" workbookViewId="1">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5387,103 +5637,103 @@
   <sheetData>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
@@ -5500,94 +5750,109 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP($A18,Table35[#All],2,TRUE)</f>
+        <v>*I</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <f>VLOOKUP($A18,Table35[#All],3,TRUE)</f>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>129</v>
+        <f>VLOOKUP($A18,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <f>VLOOKUP($A18,Table35[#All],5,TRUE)</f>
+        <v>Create Protogame as starting place</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <f>VLOOKUP($A18,Table35[#All],6,TRUE)</f>
+        <v>37</v>
       </c>
       <c r="G18" t="str">
         <f>VLOOKUP($F18,Table1[],2,TRUE)</f>
-        <v>Loading Screen</v>
+        <v>Game</v>
       </c>
       <c r="H18" t="str">
         <f>VLOOKUP($F18,Table1[],3,TRUE)</f>
-        <v>Function</v>
+        <v>Protogame</v>
       </c>
       <c r="I18" t="str">
         <f>VLOOKUP($F18,Table1[],4,TRUE)</f>
-        <v>Load data</v>
+        <v>Protogame</v>
       </c>
       <c r="J18" t="str">
         <f>VLOOKUP($F18,Table1[],5,TRUE)</f>
-        <v xml:space="preserve">Loads game assets </v>
+        <v>Create Protogame as starting point</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP($A19,Table35[#All],2,TRUE)</f>
+        <v>*0</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <f>VLOOKUP($A19,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>131</v>
+        <f>VLOOKUP($A19,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <f>VLOOKUP($A19,Table35[#All],5,TRUE)</f>
+        <v>Create simple Enemy character with functions to shoot</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <f>VLOOKUP($A19,Table35[#All],6,TRUE)</f>
+        <v>27</v>
       </c>
       <c r="G19" t="str">
         <f>VLOOKUP($F19,Table1[],2,TRUE)</f>
-        <v>Main Menu</v>
+        <v>Game</v>
       </c>
       <c r="H19" t="str">
         <f>VLOOKUP($F19,Table1[],3,TRUE)</f>
-        <v>Function</v>
+        <v>Enemies</v>
       </c>
       <c r="I19" t="str">
         <f>VLOOKUP($F19,Table1[],4,TRUE)</f>
-        <v>Buttons</v>
+        <v>Enemy characters</v>
       </c>
       <c r="J19" t="str">
         <f>VLOOKUP($F19,Table1[],5,TRUE)</f>
-        <v>Start game, Exit Game buttons to start or exit the game</v>
+        <v>Enemies are actors that may be data driven. They have on hit and on death effects to drop loot</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP($A20,Table35[#All],2,TRUE)</f>
+        <v>*0</v>
       </c>
       <c r="C20">
-        <v>1.5</v>
+        <f>VLOOKUP($A20,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>136</v>
+        <f>VLOOKUP($A20,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" t="str">
+        <f>VLOOKUP($A20,Table35[#All],5,TRUE)</f>
+        <v>Create Prototype player</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <f>VLOOKUP($A20,Table35[#All],6,TRUE)</f>
+        <v>20</v>
       </c>
       <c r="G20" t="str">
         <f>VLOOKUP($F20,Table1[],2,TRUE)</f>
@@ -5595,34 +5860,39 @@
       </c>
       <c r="H20" t="str">
         <f>VLOOKUP($F20,Table1[],3,TRUE)</f>
-        <v>Weapons</v>
+        <v>Player</v>
       </c>
       <c r="I20" t="str">
         <f>VLOOKUP($F20,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Player Character</v>
       </c>
       <c r="J20" t="str">
         <f>VLOOKUP($F20,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>The Player character is derived from actor with a player controller</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP($A21,Table35[#All],2,TRUE)</f>
+        <v>*0</v>
       </c>
       <c r="C21">
+        <f>VLOOKUP($A21,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>137</v>
+        <f>VLOOKUP($A21,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" t="str">
+        <f>VLOOKUP($A21,Table35[#All],5,TRUE)</f>
+        <v>Create prototype gun</v>
       </c>
       <c r="F21">
+        <f>VLOOKUP($A21,Table35[#All],6,TRUE)</f>
         <v>7</v>
       </c>
       <c r="G21" t="str">
@@ -5635,31 +5905,36 @@
       </c>
       <c r="I21" t="str">
         <f>VLOOKUP($F21,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Weapons</v>
       </c>
       <c r="J21" t="str">
         <f>VLOOKUP($F21,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>11</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP($A22,Table35[#All],2,TRUE)</f>
+        <v>*0</v>
       </c>
       <c r="C22">
+        <f>VLOOKUP($A22,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>140</v>
+        <f>VLOOKUP($A22,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" t="str">
+        <f>VLOOKUP($A22,Table35[#All],5,TRUE)</f>
+        <v>Create Prototype bullets/firing</v>
       </c>
       <c r="F22">
-        <v>7</v>
+        <f>VLOOKUP($A22,Table35[#All],6,TRUE)</f>
+        <v>8</v>
       </c>
       <c r="G22" t="str">
         <f>VLOOKUP($F22,Table1[],2,TRUE)</f>
@@ -5671,103 +5946,118 @@
       </c>
       <c r="I22" t="str">
         <f>VLOOKUP($F22,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Bullets</v>
       </c>
       <c r="J22" t="str">
         <f>VLOOKUP($F22,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B23">
+        <f>VLOOKUP($A23,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C23">
-        <v>1.5</v>
+        <f>VLOOKUP($A23,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" t="s">
-        <v>139</v>
+        <f>VLOOKUP($A23,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" t="str">
+        <f>VLOOKUP($A23,Table35[#All],5,TRUE)</f>
+        <v>Implement loading state and loading functions</v>
       </c>
       <c r="F23">
-        <v>7</v>
+        <f>VLOOKUP($A23,Table35[#All],6,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="G23" t="str">
         <f>VLOOKUP($F23,Table1[],2,TRUE)</f>
-        <v>Game</v>
+        <v>Loading Screen</v>
       </c>
       <c r="H23" t="str">
         <f>VLOOKUP($F23,Table1[],3,TRUE)</f>
-        <v>Weapons</v>
+        <v>Function</v>
       </c>
       <c r="I23" t="str">
         <f>VLOOKUP($F23,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Load data</v>
       </c>
       <c r="J23" t="str">
         <f>VLOOKUP($F23,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v xml:space="preserve">Loads game assets </v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B24">
+        <f>VLOOKUP($A24,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <f>VLOOKUP($A24,Table35[#All],3,TRUE)</f>
+        <v>0.5</v>
       </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>141</v>
+        <f>VLOOKUP($A24,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" t="str">
+        <f>VLOOKUP($A24,Table35[#All],5,TRUE)</f>
+        <v>Add Start button to begin the first level and exit button to quit game</v>
       </c>
       <c r="F24">
-        <v>7</v>
+        <f>VLOOKUP($A24,Table35[#All],6,TRUE)</f>
+        <v>3</v>
       </c>
       <c r="G24" t="str">
         <f>VLOOKUP($F24,Table1[],2,TRUE)</f>
-        <v>Game</v>
+        <v>Main Menu</v>
       </c>
       <c r="H24" t="str">
         <f>VLOOKUP($F24,Table1[],3,TRUE)</f>
-        <v>Weapons</v>
+        <v>Function</v>
       </c>
       <c r="I24" t="str">
         <f>VLOOKUP($F24,Table1[],4,TRUE)</f>
-        <v>Data driven Weapons</v>
+        <v>Buttons</v>
       </c>
       <c r="J24" t="str">
         <f>VLOOKUP($F24,Table1[],5,TRUE)</f>
-        <v>Weapons are data driven with Weapon visual, VFX, and SFX</v>
+        <v>Start game, Exit Game buttons to start or exit the game</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B25">
+        <f>VLOOKUP($A25,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C25">
-        <v>1.5</v>
+        <f>VLOOKUP($A25,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>145</v>
+        <f>VLOOKUP($A25,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" t="str">
+        <f>VLOOKUP($A25,Table35[#All],5,TRUE)</f>
+        <v>Integrate Weapons with bullets</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <f>VLOOKUP($A25,Table35[#All],6,TRUE)</f>
+        <v>7</v>
       </c>
       <c r="G25" t="str">
         <f>VLOOKUP($F25,Table1[],2,TRUE)</f>
@@ -5779,28 +6069,36 @@
       </c>
       <c r="I25" t="str">
         <f>VLOOKUP($F25,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Weapons</v>
       </c>
       <c r="J25" t="str">
         <f>VLOOKUP($F25,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <f>VLOOKUP($A26,Table35[#All],2,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <f>VLOOKUP($A26,Table35[#All],3,TRUE)</f>
+        <v>1.5</v>
       </c>
       <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26" t="s">
-        <v>147</v>
+        <f>VLOOKUP($A26,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" t="str">
+        <f>VLOOKUP($A26,Table35[#All],5,TRUE)</f>
+        <v>Integrate Weapon with actors</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <f>VLOOKUP($A26,Table35[#All],6,TRUE)</f>
+        <v>7</v>
       </c>
       <c r="G26" t="str">
         <f>VLOOKUP($F26,Table1[],2,TRUE)</f>
@@ -5812,31 +6110,36 @@
       </c>
       <c r="I26" t="str">
         <f>VLOOKUP($F26,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Weapons</v>
       </c>
       <c r="J26" t="str">
         <f>VLOOKUP($F26,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B27">
+        <f>VLOOKUP($A27,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C27">
+        <f>VLOOKUP($A27,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27" t="s">
-        <v>146</v>
+        <f>VLOOKUP($A27,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" t="str">
+        <f>VLOOKUP($A27,Table35[#All],5,TRUE)</f>
+        <v>Find/implement first 2 weapon assets (pistol/shotgun)</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <f>VLOOKUP($A27,Table35[#All],6,TRUE)</f>
+        <v>7</v>
       </c>
       <c r="G27" t="str">
         <f>VLOOKUP($F27,Table1[],2,TRUE)</f>
@@ -5848,31 +6151,36 @@
       </c>
       <c r="I27" t="str">
         <f>VLOOKUP($F27,Table1[],4,TRUE)</f>
-        <v>Data driven Bullets</v>
+        <v>Weapons</v>
       </c>
       <c r="J27" t="str">
         <f>VLOOKUP($F27,Table1[],5,TRUE)</f>
-        <v>Bullets are data driven with damage, visuals, VFX, and SFX</v>
+        <v>Weapons may be data driven with Weapon visual, VFX, and SFX</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B28">
+        <f>VLOOKUP($A28,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C28">
+        <f>VLOOKUP($A28,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>149</v>
+        <f>VLOOKUP($A28,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" t="str">
+        <f>VLOOKUP($A28,Table35[#All],5,TRUE)</f>
+        <v>Implement bullet collisions</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <f>VLOOKUP($A28,Table35[#All],6,TRUE)</f>
+        <v>8</v>
       </c>
       <c r="G28" t="str">
         <f>VLOOKUP($F28,Table1[],2,TRUE)</f>
@@ -5880,32 +6188,40 @@
       </c>
       <c r="H28" t="str">
         <f>VLOOKUP($F28,Table1[],3,TRUE)</f>
-        <v>Camera</v>
+        <v>Weapons</v>
       </c>
       <c r="I28" t="str">
         <f>VLOOKUP($F28,Table1[],4,TRUE)</f>
-        <v>Top down camera</v>
+        <v>Bullets</v>
       </c>
       <c r="J28" t="str">
         <f>VLOOKUP($F28,Table1[],5,TRUE)</f>
-        <v>Camera view is top down focusing on the player but is clamped to screen</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <f>VLOOKUP($A29,Table35[#All],2,TRUE)</f>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>0.5</v>
+        <f>VLOOKUP($A29,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>150</v>
+        <f>VLOOKUP($A29,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <f>VLOOKUP($A29,Table35[#All],5,TRUE)</f>
+        <v>Find/implement basic bullet asset</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <f>VLOOKUP($A29,Table35[#All],6,TRUE)</f>
+        <v>8</v>
       </c>
       <c r="G29" t="str">
         <f>VLOOKUP($F29,Table1[],2,TRUE)</f>
@@ -5913,35 +6229,40 @@
       </c>
       <c r="H29" t="str">
         <f>VLOOKUP($F29,Table1[],3,TRUE)</f>
-        <v>Camera</v>
+        <v>Weapons</v>
       </c>
       <c r="I29" t="str">
         <f>VLOOKUP($F29,Table1[],4,TRUE)</f>
-        <v>Top down camera</v>
+        <v>Bullets</v>
       </c>
       <c r="J29" t="str">
         <f>VLOOKUP($F29,Table1[],5,TRUE)</f>
-        <v>Camera view is top down focusing on the player but is clamped to screen</v>
+        <v>Bullets may be data driven with damage, visuals, VFX, and SFX</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B30">
+        <f>VLOOKUP($A30,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C30">
+        <f>VLOOKUP($A30,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>161</v>
+        <f>VLOOKUP($A30,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <f>VLOOKUP($A30,Table35[#All],5,TRUE)</f>
+        <v>Create camera to follow player</v>
       </c>
       <c r="F30">
-        <v>17</v>
+        <f>VLOOKUP($A30,Table35[#All],6,TRUE)</f>
+        <v>9</v>
       </c>
       <c r="G30" t="str">
         <f>VLOOKUP($F30,Table1[],2,TRUE)</f>
@@ -5949,35 +6270,40 @@
       </c>
       <c r="H30" t="str">
         <f>VLOOKUP($F30,Table1[],3,TRUE)</f>
-        <v>Actors</v>
+        <v>Camera</v>
       </c>
       <c r="I30" t="str">
         <f>VLOOKUP($F30,Table1[],4,TRUE)</f>
-        <v>Physics</v>
+        <v>Top down camera</v>
       </c>
       <c r="J30" t="str">
         <f>VLOOKUP($F30,Table1[],5,TRUE)</f>
-        <v>Physics like actor radius is data driven and says what the actor will collide with</v>
+        <v>Camera view is top down focusing on the player but is clamped to screen</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B31">
+        <f>VLOOKUP($A31,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <f>VLOOKUP($A31,Table35[#All],3,TRUE)</f>
+        <v>0.5</v>
       </c>
       <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31" t="s">
-        <v>158</v>
+        <f>VLOOKUP($A31,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" t="str">
+        <f>VLOOKUP($A31,Table35[#All],5,TRUE)</f>
+        <v>Clamp camera to map dimensions</v>
       </c>
       <c r="F31">
-        <v>18</v>
+        <f>VLOOKUP($A31,Table35[#All],6,TRUE)</f>
+        <v>9</v>
       </c>
       <c r="G31" t="str">
         <f>VLOOKUP($F31,Table1[],2,TRUE)</f>
@@ -5985,35 +6311,40 @@
       </c>
       <c r="H31" t="str">
         <f>VLOOKUP($F31,Table1[],3,TRUE)</f>
-        <v>Actors</v>
+        <v>Camera</v>
       </c>
       <c r="I31" t="str">
         <f>VLOOKUP($F31,Table1[],4,TRUE)</f>
-        <v>Weapons</v>
+        <v>Top down camera</v>
       </c>
       <c r="J31" t="str">
         <f>VLOOKUP($F31,Table1[],5,TRUE)</f>
-        <v>Game keeps track of current weapon and uses the weapon definitions to know the stats</v>
+        <v>Camera view is top down focusing on the player but is clamped to screen</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32">
+        <f>VLOOKUP($A32,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C32">
+        <f>VLOOKUP($A32,Table35[#All],3,TRUE)</f>
         <v>1</v>
       </c>
       <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32" t="s">
-        <v>159</v>
+        <f>VLOOKUP($A32,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <f>VLOOKUP($A32,Table35[#All],5,TRUE)</f>
+        <v>Implement Actor physics with collisions of enemies and obstacles</v>
       </c>
       <c r="F32">
-        <v>18</v>
+        <f>VLOOKUP($A32,Table35[#All],6,TRUE)</f>
+        <v>17</v>
       </c>
       <c r="G32" t="str">
         <f>VLOOKUP($F32,Table1[],2,TRUE)</f>
@@ -6025,31 +6356,36 @@
       </c>
       <c r="I32" t="str">
         <f>VLOOKUP($F32,Table1[],4,TRUE)</f>
-        <v>Weapons</v>
+        <v>Physics</v>
       </c>
       <c r="J32" t="str">
         <f>VLOOKUP($F32,Table1[],5,TRUE)</f>
-        <v>Game keeps track of current weapon and uses the weapon definitions to know the stats</v>
+        <v>Physics like actor radius is data driven and says what the actor will collide with</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33">
+        <f>VLOOKUP($A33,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C33">
-        <v>1.5</v>
+        <f>VLOOKUP($A33,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" t="s">
-        <v>160</v>
+        <f>VLOOKUP($A33,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" t="str">
+        <f>VLOOKUP($A33,Table35[#All],5,TRUE)</f>
+        <v>Have weapons face actor direction moving in a circular motion around player radius</v>
       </c>
       <c r="F33">
-        <v>19</v>
+        <f>VLOOKUP($A33,Table35[#All],6,TRUE)</f>
+        <v>18</v>
       </c>
       <c r="G33" t="str">
         <f>VLOOKUP($F33,Table1[],2,TRUE)</f>
@@ -6061,31 +6397,36 @@
       </c>
       <c r="I33" t="str">
         <f>VLOOKUP($F33,Table1[],4,TRUE)</f>
-        <v>Model/animations</v>
+        <v>Weapons</v>
       </c>
       <c r="J33" t="str">
         <f>VLOOKUP($F33,Table1[],5,TRUE)</f>
-        <v>Actors model and animations are data driven with walking and death</v>
+        <v>Game keeps track of current weapon and uses the weapon definitions to know the stats</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34">
+        <f>VLOOKUP($A34,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C34">
-        <v>1.5</v>
+        <f>VLOOKUP($A34,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34" t="s">
-        <v>162</v>
+        <f>VLOOKUP($A34,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" t="str">
+        <f>VLOOKUP($A34,Table35[#All],5,TRUE)</f>
+        <v>Have weapons behind player at top of screen and in front of player at bottom of screen</v>
       </c>
       <c r="F34">
-        <v>19</v>
+        <f>VLOOKUP($A34,Table35[#All],6,TRUE)</f>
+        <v>18</v>
       </c>
       <c r="G34" t="str">
         <f>VLOOKUP($F34,Table1[],2,TRUE)</f>
@@ -6097,31 +6438,36 @@
       </c>
       <c r="I34" t="str">
         <f>VLOOKUP($F34,Table1[],4,TRUE)</f>
-        <v>Model/animations</v>
+        <v>Weapons</v>
       </c>
       <c r="J34" t="str">
         <f>VLOOKUP($F34,Table1[],5,TRUE)</f>
-        <v>Actors model and animations are data driven with walking and death</v>
+        <v>Game keeps track of current weapon and uses the weapon definitions to know the stats</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B35">
+        <f>VLOOKUP($A35,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C35">
-        <v>1.5</v>
+        <f>VLOOKUP($A35,Table35[#All],3,TRUE)</f>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>163</v>
+        <f>VLOOKUP($A35,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" t="str">
+        <f>VLOOKUP($A35,Table35[#All],5,TRUE)</f>
+        <v>Add movement keys to controller class</v>
       </c>
       <c r="F35">
-        <v>20</v>
+        <f>VLOOKUP($A35,Table35[#All],6,TRUE)</f>
+        <v>21</v>
       </c>
       <c r="G35" t="str">
         <f>VLOOKUP($F35,Table1[],2,TRUE)</f>
@@ -6129,35 +6475,40 @@
       </c>
       <c r="H35" t="str">
         <f>VLOOKUP($F35,Table1[],3,TRUE)</f>
-        <v>Player</v>
+        <v>Player Controller</v>
       </c>
       <c r="I35" t="str">
         <f>VLOOKUP($F35,Table1[],4,TRUE)</f>
-        <v>Player Character</v>
+        <v>Movement</v>
       </c>
       <c r="J35" t="str">
         <f>VLOOKUP($F35,Table1[],5,TRUE)</f>
-        <v>The Player character is derived from actor with a player controller</v>
+        <v>Player moves with WASD or controller left joystick</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B36">
+        <f>VLOOKUP($A36,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <f>VLOOKUP($A36,Table35[#All],3,TRUE)</f>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" t="s">
-        <v>164</v>
+        <f>VLOOKUP($A36,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" t="str">
+        <f>VLOOKUP($A36,Table35[#All],5,TRUE)</f>
+        <v>Create simple enemy controller to run at player and shoot</v>
       </c>
       <c r="F36">
-        <v>21</v>
+        <f>VLOOKUP($A36,Table35[#All],6,TRUE)</f>
+        <v>28</v>
       </c>
       <c r="G36" t="str">
         <f>VLOOKUP($F36,Table1[],2,TRUE)</f>
@@ -6165,35 +6516,40 @@
       </c>
       <c r="H36" t="str">
         <f>VLOOKUP($F36,Table1[],3,TRUE)</f>
-        <v>Player Controller</v>
+        <v>Enemy Controller</v>
       </c>
       <c r="I36" t="str">
         <f>VLOOKUP($F36,Table1[],4,TRUE)</f>
-        <v>Movement</v>
+        <v>Enemy AI Controller</v>
       </c>
       <c r="J36" t="str">
         <f>VLOOKUP($F36,Table1[],5,TRUE)</f>
-        <v>Player moves with WASD or controller left joystick</v>
+        <v>Enemies have a data driven controller where they will wander until the player is spotted before chasing and shooting</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B37">
+        <f>VLOOKUP($A37,Table35[#All],2,TRUE)</f>
         <v>0</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <f>VLOOKUP($A37,Table35[#All],3,TRUE)</f>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>165</v>
+        <f>VLOOKUP($A37,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" t="str">
+        <f>VLOOKUP($A37,Table35[#All],5,TRUE)</f>
+        <v>Integrate map with actors and check collisions</v>
       </c>
       <c r="F37">
-        <v>21</v>
+        <f>VLOOKUP($A37,Table35[#All],6,TRUE)</f>
+        <v>33</v>
       </c>
       <c r="G37" t="str">
         <f>VLOOKUP($F37,Table1[],2,TRUE)</f>
@@ -6201,233 +6557,103 @@
       </c>
       <c r="H37" t="str">
         <f>VLOOKUP($F37,Table1[],3,TRUE)</f>
-        <v>Player Controller</v>
+        <v>Map</v>
       </c>
       <c r="I37" t="str">
         <f>VLOOKUP($F37,Table1[],4,TRUE)</f>
-        <v>Movement</v>
+        <v>Map makeup</v>
       </c>
       <c r="J37" t="str">
         <f>VLOOKUP($F37,Table1[],5,TRUE)</f>
-        <v>Player moves with WASD or controller left joystick</v>
+        <v>Maps are tile based with tile definitions determining what/who they block or not block</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>38</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
       <c r="C38">
-        <v>1</v>
+        <f>SUM(Table356[Estimate])</f>
+        <v>25.5</v>
       </c>
       <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>166</v>
-      </c>
-      <c r="F38">
-        <v>22</v>
-      </c>
-      <c r="G38" t="str">
-        <f>VLOOKUP($F38,Table1[],2,TRUE)</f>
-        <v>Game</v>
-      </c>
-      <c r="H38" t="str">
-        <f>VLOOKUP($F38,Table1[],3,TRUE)</f>
-        <v>Player Controller</v>
-      </c>
-      <c r="I38" t="str">
-        <f>VLOOKUP($F38,Table1[],4,TRUE)</f>
-        <v>Shooting</v>
-      </c>
-      <c r="J38" t="str">
-        <f>VLOOKUP($F38,Table1[],5,TRUE)</f>
-        <v>Player shoots with left mouse button or controller right button</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>167</v>
-      </c>
-      <c r="F39">
-        <v>23</v>
-      </c>
-      <c r="G39" t="str">
-        <f>VLOOKUP($F39,Table1[],2,TRUE)</f>
-        <v>Game</v>
-      </c>
-      <c r="H39" t="str">
-        <f>VLOOKUP($F39,Table1[],3,TRUE)</f>
-        <v>Player Controller</v>
-      </c>
-      <c r="I39" t="str">
-        <f>VLOOKUP($F39,Table1[],4,TRUE)</f>
-        <v>Aiming</v>
-      </c>
-      <c r="J39" t="str">
-        <f>VLOOKUP($F39,Table1[],5,TRUE)</f>
-        <v>Player aims with mouse or controller right joystick</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>43</v>
-      </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
+        <f>SUM(Table356[Actual])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="10">
+        <v>44011</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" t="s">
+        <v>15</v>
+      </c>
+      <c r="J42" t="s">
         <v>2</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>171</v>
-      </c>
-      <c r="F40">
-        <v>27</v>
-      </c>
-      <c r="G40" t="str">
-        <f>VLOOKUP($F40,Table1[],2,TRUE)</f>
-        <v>Game</v>
-      </c>
-      <c r="H40" t="str">
-        <f>VLOOKUP($F40,Table1[],3,TRUE)</f>
-        <v>Enemies</v>
-      </c>
-      <c r="I40" t="str">
-        <f>VLOOKUP($F40,Table1[],4,TRUE)</f>
-        <v>Enemy characters</v>
-      </c>
-      <c r="J40" t="str">
-        <f>VLOOKUP($F40,Table1[],5,TRUE)</f>
-        <v>Enemies are actors with data driven types. They have on hit and on death effects to drop loot</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>44</v>
-      </c>
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>172</v>
-      </c>
-      <c r="F41">
-        <v>28</v>
-      </c>
-      <c r="G41" t="str">
-        <f>VLOOKUP($F41,Table1[],2,TRUE)</f>
-        <v>Game</v>
-      </c>
-      <c r="H41" t="str">
-        <f>VLOOKUP($F41,Table1[],3,TRUE)</f>
-        <v>Enemy Controller</v>
-      </c>
-      <c r="I41" t="str">
-        <f>VLOOKUP($F41,Table1[],4,TRUE)</f>
-        <v>Enemy AI Controller</v>
-      </c>
-      <c r="J41" t="str">
-        <f>VLOOKUP($F41,Table1[],5,TRUE)</f>
-        <v>Enemies have a data driven controller where they will wander until the player is spotted before chasing and shooting</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>54</v>
-      </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>5</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>182</v>
-      </c>
-      <c r="F42">
-        <v>33</v>
-      </c>
-      <c r="G42" t="str">
-        <f>VLOOKUP($F42,Table1[],2,TRUE)</f>
-        <v>Game</v>
-      </c>
-      <c r="H42" t="str">
-        <f>VLOOKUP($F42,Table1[],3,TRUE)</f>
-        <v>Map</v>
-      </c>
-      <c r="I42" t="str">
-        <f>VLOOKUP($F42,Table1[],4,TRUE)</f>
-        <v>Map makeup</v>
-      </c>
-      <c r="J42" t="str">
-        <f>VLOOKUP($F42,Table1[],5,TRUE)</f>
-        <v>Maps are tile based with tile definitions determining what/who they block or not block</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <f>SUM(Table356[Estimate])</f>
-        <v>33</v>
-      </c>
-      <c r="D43">
-        <f>SUM(Table356[Actual])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="10">
-        <v>44011</v>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f>SUM(Table3567[Estimate])</f>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f>SUM(Table3567[Actual])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="2">
+        <v>44025</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E47" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F47" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G47" t="s">
         <v>14</v>
@@ -6444,40 +6670,40 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C49">
-        <f>SUM(Table3567[Estimate])</f>
+        <f>SUM(Table35678[Estimate])</f>
         <v>0</v>
       </c>
       <c r="D49">
-        <f>SUM(Table3567[Actual])</f>
+        <f>SUM(Table35678[Actual])</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B51" s="2">
-        <v>44025</v>
+        <v>44033</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E52" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F52" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G52" t="s">
         <v>14</v>
@@ -6494,60 +6720,10 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C54">
-        <f>SUM(Table35678[Estimate])</f>
+        <f>SUM(Table356789[Estimate])</f>
         <v>0</v>
       </c>
       <c r="D54">
-        <f>SUM(Table35678[Actual])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="2">
-        <v>44033</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" t="s">
-        <v>126</v>
-      </c>
-      <c r="C57" t="s">
-        <v>127</v>
-      </c>
-      <c r="D57" t="s">
-        <v>128</v>
-      </c>
-      <c r="E57" t="s">
-        <v>125</v>
-      </c>
-      <c r="F57" t="s">
-        <v>97</v>
-      </c>
-      <c r="G57" t="s">
-        <v>14</v>
-      </c>
-      <c r="H57" t="s">
-        <v>6</v>
-      </c>
-      <c r="I57" t="s">
-        <v>15</v>
-      </c>
-      <c r="J57" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C59">
-        <f>SUM(Table356789[Estimate])</f>
-        <v>0</v>
-      </c>
-      <c r="D59">
         <f>SUM(Table356789[Actual])</f>
         <v>0</v>
       </c>
@@ -6565,121 +6741,126 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734CCCA4-3ECC-40E0-914B-329F4B230DBE}">
-  <dimension ref="A2:K15"/>
+  <dimension ref="A2:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>14</v>
@@ -6699,22 +6880,22 @@
         <v>43977</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E12" s="6">
         <v>3</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H12" s="6" t="e">
         <f>VLOOKUP($G12,Table1[],2,TRUE)</f>
@@ -6738,22 +6919,22 @@
         <v>43982</v>
       </c>
       <c r="B13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E13">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H13" s="6" t="e">
         <f>VLOOKUP($G13,Table1[],2,TRUE)</f>
@@ -6777,22 +6958,22 @@
         <v>43982</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H14" s="6" t="e">
         <f>VLOOKUP($G14,Table1[],2,TRUE)</f>
@@ -6816,22 +6997,22 @@
         <v>43982</v>
       </c>
       <c r="B15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E15">
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H15" s="6" t="e">
         <f>VLOOKUP($G15,Table1[],2,TRUE)</f>
@@ -6848,6 +7029,89 @@
       <c r="K15" s="7" t="e">
         <f>VLOOKUP($G15,Table1[],5,TRUE)</f>
         <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16">
+        <v>0.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H16" s="6" t="e">
+        <f>VLOOKUP($G16,Table1[],2,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I16" s="6" t="e">
+        <f>VLOOKUP($G16,Table1[],3,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="6" t="e">
+        <f>VLOOKUP($G16,Table1[],4,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K16" s="7" t="e">
+        <f>VLOOKUP($G16,Table1[],5,TRUE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B17">
+        <v>65</v>
+      </c>
+      <c r="C17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],2,TRUE)</f>
+        <v>*I</v>
+      </c>
+      <c r="D17">
+        <f>VLOOKUP($B17,Table35[#All],3,TRUE)</f>
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f>VLOOKUP($B17,Table35[#All],4,TRUE)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],5,TRUE)</f>
+        <v>Create Protogame as starting place</v>
+      </c>
+      <c r="G17">
+        <f>VLOOKUP($B17,Table35[#All],6,TRUE)</f>
+        <v>37</v>
+      </c>
+      <c r="H17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],7,TRUE)</f>
+        <v>Game</v>
+      </c>
+      <c r="I17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],8,TRUE)</f>
+        <v>Protogame</v>
+      </c>
+      <c r="J17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],9,TRUE)</f>
+        <v>Protogame</v>
+      </c>
+      <c r="K17" t="str">
+        <f>VLOOKUP($B17,Table35[#All],10,TRUE)</f>
+        <v>Create Protogame as starting point</v>
       </c>
     </row>
   </sheetData>

</xml_diff>